<commit_message>
catching any updates not saved
</commit_message>
<xml_diff>
--- a/files/Stripped-Data/BIBB_appended.xlsx
+++ b/files/Stripped-Data/BIBB_appended.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>BM</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Precinct</t>
+  </si>
+  <si>
+    <t>BIBB-nan</t>
   </si>
   <si>
     <t>BIBB-88888</t>
@@ -647,7 +650,9 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B2">
         <v>1</v>
       </c>
@@ -729,7 +734,7 @@
     </row>
     <row r="3" spans="1:27">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -812,7 +817,7 @@
     </row>
     <row r="4" spans="1:27">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -895,7 +900,7 @@
     </row>
     <row r="5" spans="1:27">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>863</v>
@@ -978,7 +983,7 @@
     </row>
     <row r="6" spans="1:27">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>1293</v>
@@ -1061,7 +1066,7 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>696</v>
@@ -1144,7 +1149,7 @@
     </row>
     <row r="8" spans="1:27">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>794</v>
@@ -1227,7 +1232,7 @@
     </row>
     <row r="9" spans="1:27">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>672</v>
@@ -1310,7 +1315,7 @@
     </row>
     <row r="10" spans="1:27">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>2019</v>
@@ -1393,7 +1398,7 @@
     </row>
     <row r="11" spans="1:27">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>733</v>
@@ -1476,7 +1481,7 @@
     </row>
     <row r="12" spans="1:27">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>1074</v>
@@ -1559,7 +1564,7 @@
     </row>
     <row r="13" spans="1:27">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>657</v>
@@ -1642,7 +1647,7 @@
     </row>
     <row r="14" spans="1:27">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>1427</v>
@@ -1725,7 +1730,7 @@
     </row>
     <row r="15" spans="1:27">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>1063</v>
@@ -1808,7 +1813,7 @@
     </row>
     <row r="16" spans="1:27">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>572</v>
@@ -1891,7 +1896,7 @@
     </row>
     <row r="17" spans="1:27">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>1651</v>
@@ -1974,7 +1979,7 @@
     </row>
     <row r="18" spans="1:27">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18">
         <v>177</v>
@@ -2057,7 +2062,7 @@
     </row>
     <row r="19" spans="1:27">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B19">
         <v>278</v>
@@ -2140,7 +2145,7 @@
     </row>
     <row r="20" spans="1:27">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20">
         <v>134</v>
@@ -2223,7 +2228,7 @@
     </row>
     <row r="21" spans="1:27">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B21">
         <v>235</v>
@@ -2306,7 +2311,7 @@
     </row>
     <row r="22" spans="1:27">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22">
         <v>723</v>
@@ -2389,7 +2394,7 @@
     </row>
     <row r="23" spans="1:27">
       <c r="A23" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B23">
         <v>170</v>
@@ -2472,7 +2477,7 @@
     </row>
     <row r="24" spans="1:27">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B24">
         <v>225</v>
@@ -2555,7 +2560,7 @@
     </row>
     <row r="25" spans="1:27">
       <c r="A25" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B25">
         <v>153</v>
@@ -2638,7 +2643,7 @@
     </row>
     <row r="26" spans="1:27">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B26">
         <v>145</v>
@@ -2721,7 +2726,7 @@
     </row>
     <row r="27" spans="1:27">
       <c r="A27" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B27">
         <v>629</v>
@@ -2804,7 +2809,7 @@
     </row>
     <row r="28" spans="1:27">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B28">
         <v>325</v>
@@ -2887,7 +2892,7 @@
     </row>
     <row r="29" spans="1:27">
       <c r="A29" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B29">
         <v>613</v>
@@ -2970,7 +2975,7 @@
     </row>
     <row r="30" spans="1:27">
       <c r="A30" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B30">
         <v>508</v>
@@ -3053,7 +3058,7 @@
     </row>
     <row r="31" spans="1:27">
       <c r="A31" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B31">
         <v>1060</v>
@@ -3136,7 +3141,7 @@
     </row>
     <row r="32" spans="1:27">
       <c r="A32" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B32">
         <v>1292</v>
@@ -3219,7 +3224,7 @@
     </row>
     <row r="33" spans="1:27">
       <c r="A33" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B33">
         <v>163</v>
@@ -3302,7 +3307,7 @@
     </row>
     <row r="34" spans="1:27">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B34">
         <v>289</v>
@@ -3385,7 +3390,7 @@
     </row>
     <row r="35" spans="1:27">
       <c r="A35" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B35">
         <v>279</v>
@@ -3468,7 +3473,7 @@
     </row>
     <row r="36" spans="1:27">
       <c r="A36" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B36">
         <v>353</v>
@@ -3551,7 +3556,7 @@
     </row>
     <row r="37" spans="1:27">
       <c r="A37" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B37">
         <v>21270</v>

</xml_diff>